<commit_message>
Ook AS/ACS toegevoegd. De gele zijn de artikelen die me belangrijk lijken.
</commit_message>
<xml_diff>
--- a/Results/Parameters.xlsx
+++ b/Results/Parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Parameter\Author</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>3 * sqr(cols * rows)</t>
+  </si>
+  <si>
+    <t>Global update</t>
+  </si>
+  <si>
+    <t>Local update</t>
+  </si>
+  <si>
+    <t>Pheromone update:</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>ACS</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>not indicated</t>
   </si>
 </sst>
 </file>
@@ -108,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,9 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -425,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,7 +481,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -455,16 +490,16 @@
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -472,7 +507,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>10</v>
       </c>
       <c r="C2">
@@ -481,16 +516,16 @@
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>4</v>
       </c>
     </row>
@@ -498,7 +533,7 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
@@ -507,16 +542,16 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -524,19 +559,20 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>40</v>
       </c>
       <c r="C4">
         <v>300</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>40</v>
       </c>
+      <c r="F4" s="3"/>
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>40</v>
       </c>
     </row>
@@ -544,21 +580,24 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6">
@@ -567,16 +606,16 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -584,7 +623,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7">
@@ -593,16 +632,16 @@
       <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.05</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0.1</v>
       </c>
     </row>
@@ -610,22 +649,22 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>0.05</v>
       </c>
       <c r="C8">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>0.05</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>0.05</v>
       </c>
       <c r="G8">
         <v>0.01</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>0.05</v>
       </c>
     </row>
@@ -633,7 +672,7 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>0.1</v>
       </c>
       <c r="C9">
@@ -642,16 +681,16 @@
       <c r="D9">
         <v>0.05</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>0.1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>0.1</v>
       </c>
       <c r="G9">
         <v>0.02</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>0.1</v>
       </c>
     </row>
@@ -659,7 +698,7 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10">
@@ -668,17 +707,117 @@
       <c r="D10">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>8</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>8</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>